<commit_message>
collection and quality reports v1
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\Final_Amravati_CMS_Wadhghat3\InputData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="15870" windowHeight="5145"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>UserId</t>
   </si>
@@ -90,9 +95,6 @@
     <t>8-35</t>
   </si>
   <si>
-    <t>shritej.m</t>
-  </si>
-  <si>
     <t>KL</t>
   </si>
   <si>
@@ -100,13 +102,16 @@
   </si>
   <si>
     <t>7-3</t>
+  </si>
+  <si>
+    <t>http://testbaramatimc.ptaxcollection.com:8080/Pages/OfflinePayment.aspx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,21 +587,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
@@ -606,7 +611,7 @@
     <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -627,15 +632,15 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="7">
-        <v>123</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>18</v>
@@ -647,7 +652,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -667,19 +672,19 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="23.25">
+    <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -688,7 +693,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:7" ht="23.25">
+    <row r="9" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>3</v>
       </c>
@@ -703,7 +708,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -718,7 +723,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -733,22 +738,22 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -763,55 +768,55 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="13"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="16"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -821,7 +826,10 @@
   <mergeCells count="1">
     <mergeCell ref="A8:C8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>